<commit_message>
updatedÃ: Se aunieron las historias de usuario de coordinar y administrador en un solo archivo
</commit_message>
<xml_diff>
--- a/docs/Historias de usuario.xlsx
+++ b/docs/Historias de usuario.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Datos\ROBERTO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Datos\ROBERTO\PROYECTOS\mintic-syseducativo\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="62">
   <si>
     <t>ID</t>
   </si>
@@ -174,6 +174,42 @@
   </si>
   <si>
     <t>Como Administrador, quiero tener acceso a todas las funciones de los otros roles para poder corregir errores de mal uso y/o generar reportes</t>
+  </si>
+  <si>
+    <t>Como coordinador, quiero consultar el rendimiento por grupo de  docentes por materia para saber cual grupo no esta cumpliendo el registro de notas</t>
+  </si>
+  <si>
+    <t>Como coordinador , quiero consultar el rendimiento especifico de cada docente de cada materia para saber que profesor no esta cumpliendo el registro de notas</t>
+  </si>
+  <si>
+    <t>Como coordinador, quiero consultar la notas promedio por materia por grupo para saber el estado de eficiencia por materia</t>
+  </si>
+  <si>
+    <t>Como coordinador, quiero consultar las notas promedio  general por materia para saber el estado de eficiencia de cada asignatura</t>
+  </si>
+  <si>
+    <t>Como coordinador, quiero consultar el rendimiento por grupo especifico para saber el grado de eficiencia que ha alcanzado cada grupo</t>
+  </si>
+  <si>
+    <t>Como coordnador, quiero consultar el rendimiento por grado en general para saber el grado de eficiencia que ha alcanzado cada grado en general</t>
+  </si>
+  <si>
+    <t>HU17</t>
+  </si>
+  <si>
+    <t>HU18</t>
+  </si>
+  <si>
+    <t>HU19</t>
+  </si>
+  <si>
+    <t>HU20</t>
+  </si>
+  <si>
+    <t>HU21</t>
+  </si>
+  <si>
+    <t>HU22</t>
   </si>
 </sst>
 </file>
@@ -503,10 +539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -514,10 +550,11 @@
     <col min="1" max="1" width="11.42578125" style="2"/>
     <col min="2" max="2" width="30.7109375" style="3" customWidth="1"/>
     <col min="3" max="3" width="16.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="7.42578125" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.140625" customWidth="1"/>
+    <col min="8" max="8" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -802,6 +839,54 @@
         <v>3</v>
       </c>
     </row>
+    <row r="18" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>